<commit_message>
no changes just excel tracker sheets created
</commit_message>
<xml_diff>
--- a/excel tracker sheets/QUAR09 flags_QAQC 2024-03-04 .xlsx
+++ b/excel tracker sheets/QUAR09 flags_QAQC 2024-03-04 .xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/edeegan_nps_gov/Documents/FFIqaqc/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://doimspp-my.sharepoint.com/personal/edeegan_nps_gov/Documents/FFIqaqc/excel tracker sheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="375" documentId="11_5ECA08981DB4FD35060AD5E39078DBEA5674FEC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8163267C-8BA0-4AF6-8D9F-8B15F331C92D}"/>
+  <xr:revisionPtr revIDLastSave="376" documentId="11_5ECA08981DB4FD35060AD5E39078DBEA5674FEC8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E36331C-8106-4D0D-BAE7-D66E84DC2763}"/>
   <bookViews>
-    <workbookView xWindow="22710" yWindow="-15870" windowWidth="25440" windowHeight="15390" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22710" yWindow="-15870" windowWidth="25440" windowHeight="15390" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="QUAR09-01" sheetId="1" r:id="rId1"/>
@@ -815,14 +815,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -832,14 +825,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -865,9 +850,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1244,7 +1228,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -1261,7 +1245,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B3" t="s">
@@ -1278,7 +1262,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>97</v>
       </c>
       <c r="B4" t="s">
@@ -1295,7 +1279,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>98</v>
       </c>
       <c r="B5" t="s">
@@ -1312,7 +1296,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>99</v>
       </c>
       <c r="B6" t="s">
@@ -1329,7 +1313,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>100</v>
       </c>
       <c r="B7" t="s">
@@ -1346,7 +1330,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>101</v>
       </c>
       <c r="B8" t="s">
@@ -1363,7 +1347,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>102</v>
       </c>
       <c r="B9" t="s">
@@ -1380,7 +1364,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>103</v>
       </c>
       <c r="B10" t="s">
@@ -1397,7 +1381,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>104</v>
       </c>
       <c r="B11" t="s">
@@ -1414,7 +1398,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>105</v>
       </c>
       <c r="B12" t="s">
@@ -1431,7 +1415,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B13" t="s">
@@ -1445,7 +1429,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>106</v>
       </c>
       <c r="B14" t="s">
@@ -1459,7 +1443,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>107</v>
       </c>
       <c r="B15" t="s">
@@ -1473,7 +1457,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>108</v>
       </c>
       <c r="B16" t="s">
@@ -1487,7 +1471,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>109</v>
       </c>
       <c r="B17" t="s">
@@ -1504,7 +1488,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>110</v>
       </c>
       <c r="B18" t="s">
@@ -1521,7 +1505,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B19" t="s">
@@ -1538,7 +1522,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>112</v>
       </c>
       <c r="B20" t="s">
@@ -1555,7 +1539,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>113</v>
       </c>
       <c r="B21" t="s">
@@ -1572,7 +1556,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>114</v>
       </c>
       <c r="B22" t="s">
@@ -1589,7 +1573,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -1626,7 +1610,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>115</v>
       </c>
       <c r="B2" t="s">
@@ -1643,7 +1627,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>116</v>
       </c>
       <c r="B3" t="s">
@@ -1660,7 +1644,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B4" t="s">
@@ -1677,7 +1661,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>118</v>
       </c>
       <c r="B5" t="s">
@@ -1694,7 +1678,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>119</v>
       </c>
       <c r="B6" t="s">
@@ -1711,7 +1695,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>120</v>
       </c>
       <c r="B7" t="s">
@@ -1728,7 +1712,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>121</v>
       </c>
       <c r="B8" t="s">
@@ -1745,7 +1729,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>122</v>
       </c>
       <c r="B9" t="s">
@@ -1762,7 +1746,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -1776,7 +1760,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>123</v>
       </c>
       <c r="B11" t="s">
@@ -1790,7 +1774,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>124</v>
       </c>
       <c r="B12" t="s">
@@ -1804,7 +1788,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>125</v>
       </c>
       <c r="B13" t="s">
@@ -1854,7 +1838,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -1868,7 +1852,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>126</v>
       </c>
       <c r="B3" t="s">
@@ -1882,7 +1866,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B4" t="s">
@@ -1905,7 +1889,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:E44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B37" sqref="B36:B37"/>
     </sheetView>
   </sheetViews>
@@ -2248,7 +2232,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -2262,7 +2246,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
@@ -2279,7 +2263,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>241</v>
       </c>
       <c r="B8" t="s">
@@ -2296,7 +2280,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
@@ -2313,7 +2297,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
@@ -2327,7 +2311,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
@@ -2344,7 +2328,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
@@ -2358,7 +2342,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B13" t="s">
@@ -2411,7 +2395,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -2428,7 +2412,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B3" t="s">
@@ -2445,7 +2429,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -2462,7 +2446,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B5" t="s">
@@ -2479,7 +2463,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B6" t="s">
@@ -2496,7 +2480,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B7" t="s">
@@ -2513,7 +2497,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B8" t="s">
@@ -2530,7 +2514,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
@@ -2547,7 +2531,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B10" t="s">
@@ -2564,7 +2548,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B11" t="s">
@@ -2581,7 +2565,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B12" t="s">
@@ -2598,7 +2582,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B13" t="s">
@@ -2615,7 +2599,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B14" t="s">
@@ -2632,7 +2616,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B15" t="s">
@@ -2649,7 +2633,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>239</v>
       </c>
       <c r="B16" t="s">
@@ -2666,7 +2650,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="B17" t="s">
@@ -2683,7 +2667,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B18" t="s">
@@ -2700,7 +2684,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B19" t="s">
@@ -2717,7 +2701,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>21</v>
       </c>
       <c r="B20" t="s">
@@ -2734,7 +2718,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
@@ -2751,7 +2735,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B22" t="s">
@@ -2768,7 +2752,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B23" t="s">
@@ -2785,7 +2769,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
@@ -2799,7 +2783,7 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
@@ -2813,7 +2797,7 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
@@ -2827,7 +2811,7 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
@@ -2841,7 +2825,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
@@ -2855,7 +2839,7 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
@@ -2869,7 +2853,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
@@ -2883,7 +2867,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
@@ -2900,7 +2884,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -2937,7 +2921,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
@@ -2951,7 +2935,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B3" t="s">
@@ -2968,7 +2952,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B4" t="s">
@@ -2985,7 +2969,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B5" t="s">
@@ -3002,7 +2986,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B6" t="s">
@@ -3019,7 +3003,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B7" t="s">
@@ -3036,7 +3020,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B8" t="s">
@@ -3053,7 +3037,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B9" t="s">
@@ -3070,7 +3054,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B10" t="s">
@@ -3087,7 +3071,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B11" t="s">
@@ -3104,7 +3088,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B12" t="s">
@@ -3121,7 +3105,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B13" t="s">
@@ -3138,7 +3122,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>33</v>
       </c>
       <c r="B14" t="s">
@@ -3155,7 +3139,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B15" t="s">
@@ -3172,7 +3156,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B16" t="s">
@@ -3189,7 +3173,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B17" t="s">
@@ -3206,7 +3190,7 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B18" t="s">
@@ -3220,7 +3204,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>242</v>
       </c>
       <c r="B19" t="s">
@@ -3234,7 +3218,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B20" t="s">
@@ -3248,7 +3232,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -3285,7 +3269,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -3302,7 +3286,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
@@ -3319,7 +3303,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
       <c r="B4" t="s">
@@ -3336,7 +3320,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>40</v>
       </c>
       <c r="B5" t="s">
@@ -3353,7 +3337,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>41</v>
       </c>
       <c r="B6" t="s">
@@ -3370,7 +3354,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B7" t="s">
@@ -3387,7 +3371,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" t="s">
@@ -3404,7 +3388,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B9" t="s">
@@ -3421,7 +3405,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -3435,7 +3419,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
@@ -3452,7 +3436,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>44</v>
       </c>
       <c r="B12" t="s">
@@ -3469,7 +3453,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>45</v>
       </c>
       <c r="B13" t="s">
@@ -3495,8 +3479,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3522,7 +3506,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>46</v>
       </c>
       <c r="B2" t="s">
@@ -3539,7 +3523,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B3" t="s">
@@ -3556,7 +3540,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B4" t="s">
@@ -3573,7 +3557,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>48</v>
       </c>
       <c r="B5" t="s">
@@ -4134,7 +4118,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B38" t="s">
@@ -4148,7 +4132,7 @@
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>81</v>
       </c>
       <c r="B39" t="s">
@@ -4162,7 +4146,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>82</v>
       </c>
       <c r="B40" t="s">
@@ -4176,7 +4160,7 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>83</v>
       </c>
       <c r="B41" t="s">
@@ -4193,9 +4177,9 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4230,7 +4214,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
@@ -4280,7 +4264,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>84</v>
       </c>
       <c r="B2" t="s">
@@ -4297,7 +4281,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B3" t="s">
@@ -4314,7 +4298,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B4" t="s">
@@ -4331,7 +4315,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B5" t="s">
@@ -4345,7 +4329,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B6" t="s">
@@ -4359,7 +4343,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>85</v>
       </c>
       <c r="B7" t="s">
@@ -4373,7 +4357,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>86</v>
       </c>
       <c r="B8" t="s">
@@ -4387,7 +4371,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>87</v>
       </c>
       <c r="B9" t="s">
@@ -4401,7 +4385,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
@@ -4415,7 +4399,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>88</v>
       </c>
       <c r="B11" t="s">
@@ -4429,7 +4413,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>89</v>
       </c>
       <c r="B12" t="s">
@@ -4443,7 +4427,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>90</v>
       </c>
       <c r="B13" t="s">
@@ -4457,7 +4441,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>91</v>
       </c>
       <c r="B14" t="s">
@@ -4471,7 +4455,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>92</v>
       </c>
       <c r="B15" t="s">
@@ -4485,7 +4469,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>93</v>
       </c>
       <c r="B16" t="s">
@@ -4512,7 +4496,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A9"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4538,7 +4522,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
@@ -4555,7 +4539,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B3" t="s">
@@ -4572,7 +4556,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B4" t="s">
@@ -4589,7 +4573,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B5" t="s">
@@ -4606,7 +4590,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B6" t="s">
@@ -4623,7 +4607,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B7" t="s">
@@ -4640,7 +4624,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B8" t="s">
@@ -4657,7 +4641,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B9" t="s">
@@ -4674,7 +4658,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>240</v>
       </c>
       <c r="B10" t="s">
@@ -4691,7 +4675,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B11" t="s">
@@ -4705,7 +4689,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>95</v>
       </c>
       <c r="B12" t="s">
@@ -4719,7 +4703,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>96</v>
       </c>
       <c r="B13" t="s">
@@ -4736,7 +4720,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>

</xml_diff>